<commit_message>
Added entry for Wednesday
</commit_message>
<xml_diff>
--- a/Ticket_Tally_Sheet.xlsx
+++ b/Ticket_Tally_Sheet.xlsx
@@ -20,9 +20,9 @@
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1035" activeSheetId="3"/>
+    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
     <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="3"/>
-    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
-    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1035" activeSheetId="3"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -433,7 +433,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{2C5E94BD-335E-4AEA-9E27-FFC8F5F549F9}" diskRevisions="1" revisionId="20" version="7">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{AFBFCBDA-AB89-4BE7-8604-B1DFADC92617}" diskRevisions="1" revisionId="22" version="8">
   <header guid="{A9502BF7-CEAC-41BD-8BA9-F19A93511DBE}" dateTime="2017-09-29T21:44:11" maxSheetId="6" userName="Jeric Ryan De Josef" r:id="rId1">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -489,6 +489,15 @@
     </sheetIdMap>
   </header>
   <header guid="{2C5E94BD-335E-4AEA-9E27-FFC8F5F549F9}" dateTime="2017-10-04T03:39:37" maxSheetId="6" userName="Benson Fabonan" r:id="rId7" minRId="19" maxRId="20">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{AFBFCBDA-AB89-4BE7-8604-B1DFADC92617}" dateTime="2017-10-04T03:40:54" maxSheetId="6" userName="Benson Fabonan" r:id="rId8" minRId="21" maxRId="22">
     <sheetIdMap count="5">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -635,6 +644,21 @@
   </rcc>
   <rcc rId="20" sId="3">
     <nc r="F6">
+      <v>0</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="21" sId="3">
+    <nc r="G5">
+      <v>0</v>
+    </nc>
+  </rcc>
+  <rcc rId="22" sId="3">
+    <nc r="G6">
       <v>0</v>
     </nc>
   </rcc>
@@ -1433,7 +1457,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1443,7 +1467,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1943,7 +1967,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1953,7 +1977,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1974,7 +1998,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2074,7 +2098,9 @@
       <c r="F5" s="16">
         <v>1</v>
       </c>
-      <c r="G5" s="16"/>
+      <c r="G5" s="16">
+        <v>0</v>
+      </c>
       <c r="H5" s="16"/>
       <c r="I5" s="16">
         <f>SUM(C5:H5)</f>
@@ -2111,7 +2137,9 @@
       <c r="F6" s="16">
         <v>0</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="16">
+        <v>0</v>
+      </c>
       <c r="H6" s="16"/>
       <c r="I6" s="16">
         <f t="shared" ref="I6:I14" si="2">SUM(C6:H6)</f>
@@ -2430,13 +2458,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -2872,13 +2900,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="E10" sqref="E10"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="C13" sqref="C13:G14"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="C13" sqref="C13:G14"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="E10" sqref="E10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -3314,12 +3342,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="D25" sqref="D25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="D25" sqref="D25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Updated Entry for Friday
</commit_message>
<xml_diff>
--- a/Ticket_Tally_Sheet.xlsx
+++ b/Ticket_Tally_Sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tally_20170914" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,9 @@
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1035" activeSheetId="3"/>
+    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
     <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="3"/>
-    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
-    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1035" activeSheetId="3"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -433,7 +433,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{3E16E234-9C5F-4A1F-AE2A-F6E6846155B7}" diskRevisions="1" revisionId="24" version="9">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F5F81CB7-964F-4AE1-8957-C7E06111E093}" diskRevisions="1" revisionId="26" version="10">
   <header guid="{A9502BF7-CEAC-41BD-8BA9-F19A93511DBE}" dateTime="2017-09-29T21:44:11" maxSheetId="6" userName="Jeric Ryan De Josef" r:id="rId1">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -515,11 +515,35 @@
       <sheetId val="5"/>
     </sheetIdMap>
   </header>
+  <header guid="{F5F81CB7-964F-4AE1-8957-C7E06111E093}" dateTime="2017-10-07T05:26:51" maxSheetId="6" userName="Benson Fabonan" r:id="rId10" minRId="25" maxRId="26">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="25" sId="4">
+    <nc r="C5">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="26" sId="4">
+    <nc r="C6">
+      <v>0</v>
+    </nc>
+  </rcc>
+</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -690,11 +714,10 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="4">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="3">
   <userInfo guid="{C94F292E-DFF6-48AF-9BAB-56014F57DFC0}" name="Jeric Ryan De Josef" id="-2144758671" dateTime="2017-09-29T21:44:11"/>
   <userInfo guid="{C94F292E-DFF6-48AF-9BAB-56014F57DFC0}" name="Benson Fabonan" id="-111965015" dateTime="2017-10-04T01:23:59"/>
   <userInfo guid="{7AB22875-E732-4E6E-95B4-D451FF1B42BE}" name="Benson Fabonan" id="-111948917" dateTime="2017-10-04T01:45:45"/>
-  <userInfo guid="{3E16E234-9C5F-4A1F-AE2A-F6E6846155B7}" name="Benson Fabonan" id="-112000366" dateTime="2017-10-06T00:43:14"/>
 </users>
 </file>
 
@@ -1482,7 +1505,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1492,7 +1515,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1992,7 +2015,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2002,7 +2025,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2022,8 +2045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2487,13 +2510,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -2512,8 +2535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2601,7 +2624,9 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="16">
+        <v>2</v>
+      </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
@@ -2609,7 +2634,7 @@
       <c r="H5" s="16"/>
       <c r="I5" s="16">
         <f>SUM(C5:H5)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="24" t="s">
@@ -2630,7 +2655,9 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="16">
+        <v>0</v>
+      </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
@@ -2645,7 +2672,7 @@
       </c>
       <c r="N6" s="16">
         <f>I5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O6" s="16">
         <f>I6</f>
@@ -2764,7 +2791,7 @@
       </c>
       <c r="N9" s="16">
         <f>SUM(N6:N8)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O9" s="16">
         <f t="shared" ref="O9" si="3">SUM(O6:O8)</f>
@@ -2929,13 +2956,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="E10" sqref="E10"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="C13" sqref="C13:G14"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="C13" sqref="C13:G14"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="E10" sqref="E10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -3371,12 +3398,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="D25" sqref="D25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="D25" sqref="D25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Added my entries for 10/5 week.
</commit_message>
<xml_diff>
--- a/Ticket_Tally_Sheet.xlsx
+++ b/Ticket_Tally_Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SSIS-Shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SSIS\SSIS-Shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,12 +17,15 @@
     <sheet name="Tally_20170928" sheetId="3" r:id="rId3"/>
     <sheet name="Tally_20171005" sheetId="4" r:id="rId4"/>
     <sheet name="Tally_20171012" sheetId="5" r:id="rId5"/>
+    <sheet name="Tally_20171019" sheetId="6" r:id="rId6"/>
+    <sheet name="Tally_20171026" sheetId="7" r:id="rId7"/>
+    <sheet name="Tally_20171102" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
+    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
     <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="4"/>
-    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1035" activeSheetId="3"/>
-    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="10">
   <si>
     <t>Benson Fabonan</t>
   </si>
@@ -338,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -398,6 +401,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -430,386 +436,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{84295E03-DB4D-424E-8AE1-A592E99C7999}" diskRevisions="1" revisionId="34" version="13">
-  <header guid="{A9502BF7-CEAC-41BD-8BA9-F19A93511DBE}" dateTime="2017-09-29T21:44:11" maxSheetId="6" userName="Jeric Ryan De Josef" r:id="rId1">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{0CE68987-16A2-4A7D-B0F2-3D1072AB69BE}" dateTime="2017-09-29T22:04:49" maxSheetId="6" userName="Jeric Ryan De Josef" r:id="rId2" minRId="1" maxRId="2">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{0BA89637-022C-48A5-BDDB-9C6E916295DF}" dateTime="2017-09-30T00:03:38" maxSheetId="6" userName="Jeric Ryan De Josef" r:id="rId3" minRId="3">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{C94F292E-DFF6-48AF-9BAB-56014F57DFC0}" dateTime="2017-09-30T00:18:42" maxSheetId="6" userName="Jeric Ryan De Josef" r:id="rId4" minRId="4">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{7AB22875-E732-4E6E-95B4-D451FF1B42BE}" dateTime="2017-10-04T01:48:11" maxSheetId="6" userName="Benson Fabonan" r:id="rId5" minRId="5" maxRId="10">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{31096640-7508-4DF7-A365-2B7301ABCD9D}" dateTime="2017-10-04T03:28:55" maxSheetId="6" userName="Manuel Alberto Lomotan" r:id="rId6" minRId="11" maxRId="18">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{2C5E94BD-335E-4AEA-9E27-FFC8F5F549F9}" dateTime="2017-10-04T03:39:37" maxSheetId="6" userName="Benson Fabonan" r:id="rId7" minRId="19" maxRId="20">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{AFBFCBDA-AB89-4BE7-8604-B1DFADC92617}" dateTime="2017-10-04T03:40:54" maxSheetId="6" userName="Benson Fabonan" r:id="rId8" minRId="21" maxRId="22">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{3E16E234-9C5F-4A1F-AE2A-F6E6846155B7}" dateTime="2017-10-06T00:43:44" maxSheetId="6" userName="Benson Fabonan" r:id="rId9" minRId="23" maxRId="24">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{F5F81CB7-964F-4AE1-8957-C7E06111E093}" dateTime="2017-10-07T05:26:51" maxSheetId="6" userName="Benson Fabonan" r:id="rId10" minRId="25" maxRId="26">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{CC5FFA19-60FF-49F0-BB71-B3CB6096DA1C}" dateTime="2017-10-10T04:08:24" maxSheetId="6" userName="Benson Fabonan" r:id="rId11" minRId="27" maxRId="30">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{FAFD3C1E-D1D3-470A-B045-C1E90597F3AD}" dateTime="2017-10-10T06:18:58" maxSheetId="6" userName="Benson Fabonan" r:id="rId12" minRId="31" maxRId="32">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{84295E03-DB4D-424E-8AE1-A592E99C7999}" dateTime="2017-10-11T05:33:53" maxSheetId="6" userName="Benson Fabonan" r:id="rId13" minRId="33" maxRId="34">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-</headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="25" sId="4">
-    <nc r="C5">
-      <v>2</v>
-    </nc>
-  </rcc>
-  <rcc rId="26" sId="4">
-    <nc r="C6">
-      <v>0</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="27" sId="4">
-    <nc r="D5">
-      <v>2</v>
-    </nc>
-  </rcc>
-  <rcc rId="28" sId="4">
-    <nc r="D6">
-      <v>2</v>
-    </nc>
-  </rcc>
-  <rcc rId="29" sId="4">
-    <nc r="E5">
-      <v>0</v>
-    </nc>
-  </rcc>
-  <rcc rId="30" sId="4">
-    <nc r="E6">
-      <v>0</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="31" sId="4">
-    <oc r="E5">
-      <v>0</v>
-    </oc>
-    <nc r="E5">
-      <v>1</v>
-    </nc>
-  </rcc>
-  <rcc rId="32" sId="4">
-    <oc r="E6">
-      <v>0</v>
-    </oc>
-    <nc r="E6">
-      <v>1</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="33" sId="4">
-    <nc r="F5">
-      <v>1</v>
-    </nc>
-  </rcc>
-  <rcc rId="34" sId="4">
-    <nc r="F6">
-      <v>1</v>
-    </nc>
-  </rcc>
-  <rcv guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" action="delete"/>
-  <rcv guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1" sId="3">
-    <nc r="D9">
-      <v>1</v>
-    </nc>
-  </rcc>
-  <rcc rId="2" sId="3">
-    <nc r="D10">
-      <v>0</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="3" sId="3">
-    <oc r="D10">
-      <v>0</v>
-    </oc>
-    <nc r="D10">
-      <v>1</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="4" sId="3">
-    <oc r="D9">
-      <v>1</v>
-    </oc>
-    <nc r="D9">
-      <v>2</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="5" sId="3">
-    <nc r="C5">
-      <v>3</v>
-    </nc>
-  </rcc>
-  <rcc rId="6" sId="3">
-    <nc r="C6">
-      <v>3</v>
-    </nc>
-  </rcc>
-  <rcc rId="7" sId="3">
-    <nc r="D5">
-      <v>1</v>
-    </nc>
-  </rcc>
-  <rcc rId="8" sId="3">
-    <nc r="D6">
-      <v>0</v>
-    </nc>
-  </rcc>
-  <rcc rId="9" sId="3">
-    <nc r="E5">
-      <v>3</v>
-    </nc>
-  </rcc>
-  <rcc rId="10" sId="3">
-    <nc r="E6">
-      <v>0</v>
-    </nc>
-  </rcc>
-  <rcv guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="11" sId="3">
-    <nc r="C13">
-      <v>1</v>
-    </nc>
-  </rcc>
-  <rcc rId="12" sId="3">
-    <nc r="C14">
-      <v>1</v>
-    </nc>
-  </rcc>
-  <rcc rId="13" sId="3">
-    <nc r="D13">
-      <v>1</v>
-    </nc>
-  </rcc>
-  <rcc rId="14" sId="3">
-    <nc r="D14">
-      <v>1</v>
-    </nc>
-  </rcc>
-  <rcc rId="15" sId="3">
-    <nc r="E13">
-      <v>2</v>
-    </nc>
-  </rcc>
-  <rcc rId="16" sId="3">
-    <nc r="E14">
-      <v>0</v>
-    </nc>
-  </rcc>
-  <rcc rId="17" sId="3">
-    <nc r="F13">
-      <v>2</v>
-    </nc>
-  </rcc>
-  <rcc rId="18" sId="3">
-    <nc r="F14">
-      <v>2</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="19" sId="3">
-    <nc r="F5">
-      <v>1</v>
-    </nc>
-  </rcc>
-  <rcc rId="20" sId="3">
-    <nc r="F6">
-      <v>0</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="21" sId="3">
-    <nc r="G5">
-      <v>0</v>
-    </nc>
-  </rcc>
-  <rcc rId="22" sId="3">
-    <nc r="G6">
-      <v>0</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="23" sId="3">
-    <nc r="H5">
-      <v>2</v>
-    </nc>
-  </rcc>
-  <rcc rId="24" sId="3">
-    <nc r="H6">
-      <v>0</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="4">
-  <userInfo guid="{C94F292E-DFF6-48AF-9BAB-56014F57DFC0}" name="Jeric Ryan De Josef" id="-2144758671" dateTime="2017-09-29T21:44:11"/>
-  <userInfo guid="{C94F292E-DFF6-48AF-9BAB-56014F57DFC0}" name="Benson Fabonan" id="-111965015" dateTime="2017-10-04T01:23:59"/>
-  <userInfo guid="{7AB22875-E732-4E6E-95B4-D451FF1B42BE}" name="Benson Fabonan" id="-111948917" dateTime="2017-10-04T01:45:45"/>
-  <userInfo guid="{84295E03-DB4D-424E-8AE1-A592E99C7999}" name="Benson Fabonan" id="-111961823" dateTime="2017-10-11T05:33:27"/>
-</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1194,7 +820,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1235,7 +861,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="7" t="s">
         <v>3</v>
       </c>
@@ -1278,7 +904,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -1320,7 +946,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
@@ -1362,7 +988,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="26" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -1409,7 +1035,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="7" t="s">
         <v>3</v>
       </c>
@@ -1437,7 +1063,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="7" t="s">
         <v>4</v>
       </c>
@@ -1462,7 +1088,7 @@
       <c r="I11" s="12"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="8" t="s">
         <v>5</v>
       </c>
@@ -1487,7 +1113,7 @@
       <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="26" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -1517,7 +1143,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="7" t="s">
         <v>3</v>
       </c>
@@ -1545,7 +1171,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="7" t="s">
         <v>4</v>
       </c>
@@ -1570,7 +1196,7 @@
       <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="8" t="s">
         <v>5</v>
       </c>
@@ -1596,17 +1222,17 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1712,7 +1338,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1751,7 +1377,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1792,7 +1418,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1834,7 +1460,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1876,7 +1502,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1923,7 +1549,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1951,7 +1577,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1976,7 +1602,7 @@
       <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -2001,7 +1627,7 @@
       <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2029,7 +1655,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -2055,7 +1681,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2080,7 +1706,7 @@
       <c r="I15" s="16"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -2106,18 +1732,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="H11" sqref="H11"/>
+    <customSheetView guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}">
+      <selection activeCell="G21" sqref="G21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}">
-      <selection activeCell="G21" sqref="G21"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -2134,24 +1760,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10" customWidth="1"/>
-    <col min="16" max="17" width="19.7109375" customWidth="1"/>
+    <col min="3" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10" customWidth="1"/>
+    <col min="15" max="16" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2159,11 +1785,11 @@
         <v>43006</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C3" s="9">
         <f>B1</f>
         <v>43006</v>
@@ -2177,25 +1803,21 @@
         <v>43010</v>
       </c>
       <c r="F3" s="9">
-        <f t="shared" ref="F3:H3" si="0">E3+1</f>
+        <f t="shared" ref="F3:G3" si="0">E3+1</f>
         <v>43011</v>
       </c>
       <c r="G3" s="9">
         <f t="shared" si="0"/>
         <v>43012</v>
       </c>
-      <c r="H3" s="9">
-        <f t="shared" si="0"/>
-        <v>43013</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C4" s="10" t="str">
         <f>TEXT(C3,"DDDD")</f>
         <v>Thursday</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f t="shared" ref="D4:H4" si="1">TEXT(D3,"DDDD")</f>
+        <f t="shared" ref="D4:G4" si="1">TEXT(D3,"DDDD")</f>
         <v>Friday</v>
       </c>
       <c r="E4" s="10" t="str">
@@ -2210,16 +1832,12 @@
         <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
-      <c r="H4" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>Thursday</v>
-      </c>
-      <c r="I4" s="21" t="s">
+      <c r="H4" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2241,28 +1859,25 @@
         <v>0</v>
       </c>
       <c r="H5" s="16">
-        <v>2</v>
-      </c>
-      <c r="I5" s="16">
-        <f>SUM(C5:H5)</f>
-        <v>10</v>
-      </c>
-      <c r="M5" s="1"/>
+        <f>SUM(C5:G5)</f>
+        <v>8</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="24" t="s">
+        <v>2</v>
+      </c>
       <c r="N5" s="24" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O5" s="24" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P5" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2282,32 +1897,29 @@
         <v>0</v>
       </c>
       <c r="H6" s="16">
-        <v>0</v>
-      </c>
-      <c r="I6" s="16">
-        <f t="shared" ref="I6:I14" si="2">SUM(C6:H6)</f>
-        <v>3</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>0</v>
+        <f>SUM(C6:G6)</f>
+        <v>3</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16">
+        <f>H5</f>
+        <v>8</v>
       </c>
       <c r="N6" s="16">
-        <f>I5</f>
-        <v>10</v>
-      </c>
-      <c r="O6" s="16">
-        <f>I6</f>
-        <v>3</v>
+        <f>H6</f>
+        <v>3</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="P6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="29"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2326,30 +1938,27 @@
       <c r="G7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="16"/>
-      <c r="M7" s="5" t="s">
+      <c r="H7" s="16"/>
+      <c r="L7" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="M7" s="16">
+        <f>H9</f>
+        <v>20</v>
+      </c>
       <c r="N7" s="16">
-        <f>I9</f>
-        <v>3</v>
-      </c>
-      <c r="O7" s="16">
-        <f>I10</f>
-        <v>1</v>
+        <f>H10</f>
+        <v>15</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="P7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2368,69 +1977,71 @@
       <c r="G8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="16"/>
-      <c r="M8" s="5" t="s">
+      <c r="H8" s="16"/>
+      <c r="L8" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="M8" s="16">
+        <f>H13</f>
+        <v>10</v>
+      </c>
       <c r="N8" s="16">
-        <f>I13</f>
-        <v>6</v>
-      </c>
-      <c r="O8" s="16">
-        <f>I14</f>
+        <f>H14</f>
+        <v>5</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="16">
+        <v>2</v>
+      </c>
+      <c r="D9" s="16">
+        <v>5</v>
+      </c>
+      <c r="E9" s="16">
         <v>4</v>
       </c>
-      <c r="P8" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="16">
-        <v>1</v>
-      </c>
-      <c r="D9" s="16">
-        <v>2</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="M9" s="23" t="s">
+      <c r="F9" s="16">
+        <v>6</v>
+      </c>
+      <c r="G9" s="16">
+        <v>3</v>
+      </c>
+      <c r="H9" s="16">
+        <f>SUM(C9:G9)</f>
+        <v>20</v>
+      </c>
+      <c r="L9" s="23" t="s">
         <v>8</v>
       </c>
+      <c r="M9" s="16">
+        <f>SUM(M6:M8)</f>
+        <v>38</v>
+      </c>
       <c r="N9" s="16">
-        <f>SUM(N6:N8)</f>
-        <v>19</v>
-      </c>
-      <c r="O9" s="16">
-        <f t="shared" ref="O9" si="3">SUM(O6:O8)</f>
-        <v>8</v>
+        <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
+        <v>23</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="P9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="Q9" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -2438,19 +2049,24 @@
         <v>0</v>
       </c>
       <c r="D10" s="16">
-        <v>1</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
+        <v>2</v>
+      </c>
+      <c r="E10" s="16">
+        <v>4</v>
+      </c>
+      <c r="F10" s="16">
+        <v>3</v>
+      </c>
+      <c r="G10" s="16">
+        <v>6</v>
+      </c>
+      <c r="H10" s="16">
+        <f>SUM(C10:G10)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -2469,13 +2085,10 @@
       <c r="G11" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I11" s="16"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -2494,13 +2107,10 @@
       <c r="G12" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="16"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2518,15 +2128,16 @@
       <c r="F13" s="16">
         <v>2</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="G13" s="16">
+        <v>4</v>
+      </c>
+      <c r="H13" s="16">
+        <f>SUM(C13:G13)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -2542,15 +2153,16 @@
       <c r="F14" s="16">
         <v>2</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
+      <c r="G14" s="16">
+        <v>1</v>
+      </c>
+      <c r="H14" s="16">
+        <f>SUM(C14:G14)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2569,13 +2181,10 @@
       <c r="G15" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" s="16"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -2594,20 +2203,17 @@
       <c r="G16" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I16" s="16"/>
+      <c r="H16" s="16"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -2624,24 +2230,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10" customWidth="1"/>
-    <col min="16" max="17" width="19.7109375" customWidth="1"/>
+    <col min="3" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10" customWidth="1"/>
+    <col min="15" max="16" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2649,11 +2255,11 @@
         <v>43013</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C3" s="9">
         <f>B1</f>
         <v>43013</v>
@@ -2667,25 +2273,21 @@
         <v>43017</v>
       </c>
       <c r="F3" s="9">
-        <f t="shared" ref="F3:H3" si="0">E3+1</f>
+        <f t="shared" ref="F3:G3" si="0">E3+1</f>
         <v>43018</v>
       </c>
       <c r="G3" s="9">
         <f t="shared" si="0"/>
         <v>43019</v>
       </c>
-      <c r="H3" s="9">
-        <f t="shared" si="0"/>
-        <v>43020</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C4" s="10" t="str">
         <f>TEXT(C3,"DDDD")</f>
         <v>Thursday</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f t="shared" ref="D4:H4" si="1">TEXT(D3,"DDDD")</f>
+        <f t="shared" ref="D4:G4" si="1">TEXT(D3,"DDDD")</f>
         <v>Friday</v>
       </c>
       <c r="E4" s="10" t="str">
@@ -2700,16 +2302,12 @@
         <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
-      <c r="H4" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>Thursday</v>
-      </c>
-      <c r="I4" s="21" t="s">
+      <c r="H4" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2728,27 +2326,26 @@
         <v>1</v>
       </c>
       <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16">
-        <f>SUM(C5:H5)</f>
-        <v>6</v>
-      </c>
-      <c r="M5" s="1"/>
+      <c r="H5" s="16">
+        <f>SUM(C5:G5)</f>
+        <v>6</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="24" t="s">
+        <v>2</v>
+      </c>
       <c r="N5" s="24" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O5" s="24" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P5" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2765,31 +2362,30 @@
         <v>1</v>
       </c>
       <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16">
-        <f t="shared" ref="I6:I14" si="2">SUM(C6:H6)</f>
+      <c r="H6" s="16">
+        <f>SUM(C6:G6)</f>
         <v>4</v>
       </c>
-      <c r="M6" s="5" t="s">
-        <v>0</v>
+      <c r="L6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16">
+        <f>H5</f>
+        <v>6</v>
       </c>
       <c r="N6" s="16">
-        <f>I5</f>
-        <v>6</v>
-      </c>
-      <c r="O6" s="16">
-        <f>I6</f>
+        <f>H6</f>
         <v>4</v>
       </c>
+      <c r="O6" s="16" t="s">
+        <v>6</v>
+      </c>
       <c r="P6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="29"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2808,30 +2404,27 @@
       <c r="G7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="16"/>
-      <c r="M7" s="5" t="s">
+      <c r="H7" s="16"/>
+      <c r="L7" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="M7" s="16">
+        <f>H9</f>
+        <v>10</v>
+      </c>
       <c r="N7" s="16">
-        <f>I9</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="16">
-        <f>I10</f>
-        <v>0</v>
+        <f>H10</f>
+        <v>7</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="P7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2850,81 +2443,94 @@
       <c r="G8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="16"/>
-      <c r="M8" s="5" t="s">
+      <c r="H8" s="16"/>
+      <c r="L8" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="M8" s="16">
+        <f>H13</f>
+        <v>0</v>
+      </c>
       <c r="N8" s="16">
-        <f>I13</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="16">
-        <f>I14</f>
-        <v>0</v>
+        <f>H14</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="P8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="23" t="s">
+      <c r="C9" s="16">
+        <v>2</v>
+      </c>
+      <c r="D9" s="16">
+        <v>1</v>
+      </c>
+      <c r="E9" s="16">
+        <v>3</v>
+      </c>
+      <c r="F9" s="16">
+        <v>2</v>
+      </c>
+      <c r="G9" s="16">
+        <v>2</v>
+      </c>
+      <c r="H9" s="16">
+        <f>SUM(C9:G9)</f>
+        <v>10</v>
+      </c>
+      <c r="L9" s="23" t="s">
         <v>8</v>
       </c>
+      <c r="M9" s="16">
+        <f>SUM(M6:M8)</f>
+        <v>16</v>
+      </c>
       <c r="N9" s="16">
-        <f>SUM(N6:N8)</f>
-        <v>6</v>
-      </c>
-      <c r="O9" s="16">
-        <f t="shared" ref="O9" si="3">SUM(O6:O8)</f>
-        <v>4</v>
+        <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
+        <v>11</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="P9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="Q9" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="C10" s="16">
+        <v>3</v>
+      </c>
+      <c r="D10" s="16">
+        <v>2</v>
+      </c>
       <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
+      <c r="F10" s="16">
+        <v>1</v>
+      </c>
+      <c r="G10" s="16">
+        <v>1</v>
+      </c>
+      <c r="H10" s="16">
+        <f>SUM(C10:G10)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -2943,13 +2549,10 @@
       <c r="G11" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I11" s="16"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -2968,13 +2571,10 @@
       <c r="G12" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="16"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2985,14 +2585,13 @@
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="H13" s="16">
+        <f>SUM(C13:G13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -3001,14 +2600,13 @@
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
+      <c r="H14" s="16">
+        <f>SUM(C14:G14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -3027,13 +2625,10 @@
       <c r="G15" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" s="16"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -3052,20 +2647,17 @@
       <c r="G16" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I16" s="16"/>
+      <c r="H16" s="16"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="I31" sqref="I31"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="C13" sqref="C13:G14"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="I31" sqref="I31"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -3082,24 +2674,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="E25" sqref="E24:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10" customWidth="1"/>
-    <col min="16" max="17" width="19.7109375" customWidth="1"/>
+    <col min="3" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10" customWidth="1"/>
+    <col min="15" max="16" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3107,11 +2699,11 @@
         <v>43020</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C3" s="9">
         <f>B1</f>
         <v>43020</v>
@@ -3125,25 +2717,21 @@
         <v>43024</v>
       </c>
       <c r="F3" s="9">
-        <f t="shared" ref="F3:H3" si="0">E3+1</f>
+        <f t="shared" ref="F3:G3" si="0">E3+1</f>
         <v>43025</v>
       </c>
       <c r="G3" s="9">
         <f t="shared" si="0"/>
         <v>43026</v>
       </c>
-      <c r="H3" s="9">
-        <f t="shared" si="0"/>
-        <v>43027</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C4" s="10" t="str">
         <f>TEXT(C3,"DDDD")</f>
         <v>Thursday</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f t="shared" ref="D4:H4" si="1">TEXT(D3,"DDDD")</f>
+        <f t="shared" ref="D4:G4" si="1">TEXT(D3,"DDDD")</f>
         <v>Friday</v>
       </c>
       <c r="E4" s="10" t="str">
@@ -3158,16 +2746,12 @@
         <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
-      <c r="H4" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>Thursday</v>
-      </c>
-      <c r="I4" s="21" t="s">
+      <c r="H4" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3178,27 +2762,26 @@
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16">
-        <f>SUM(C5:H5)</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="1"/>
+      <c r="H5" s="16">
+        <f>SUM(C5:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="24" t="s">
+        <v>2</v>
+      </c>
       <c r="N5" s="24" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O5" s="24" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P5" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3207,31 +2790,30 @@
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16">
-        <f t="shared" ref="I6:I14" si="2">SUM(C6:H6)</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="5" t="s">
+      <c r="H6" s="16">
+        <f>SUM(C6:G6)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16">
+        <f>H5</f>
         <v>0</v>
       </c>
       <c r="N6" s="16">
-        <f>I5</f>
-        <v>0</v>
-      </c>
-      <c r="O6" s="16">
-        <f>I6</f>
-        <v>0</v>
+        <f>H6</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="P6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="29"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3250,30 +2832,27 @@
       <c r="G7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="16"/>
-      <c r="M7" s="5" t="s">
+      <c r="H7" s="16"/>
+      <c r="L7" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="M7" s="16">
+        <f>H9</f>
+        <v>0</v>
+      </c>
       <c r="N7" s="16">
-        <f>I9</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="16">
-        <f>I10</f>
-        <v>0</v>
+        <f>H10</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="P7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3292,30 +2871,27 @@
       <c r="G8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="16"/>
-      <c r="M8" s="5" t="s">
+      <c r="H8" s="16"/>
+      <c r="L8" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="M8" s="16">
+        <f>H13</f>
+        <v>0</v>
+      </c>
       <c r="N8" s="16">
-        <f>I13</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="16">
-        <f>I14</f>
-        <v>0</v>
+        <f>H14</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="P8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -3326,31 +2902,30 @@
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="23" t="s">
+      <c r="H9" s="16">
+        <f>SUM(C9:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="23" t="s">
         <v>8</v>
       </c>
+      <c r="M9" s="16">
+        <f>SUM(M6:M8)</f>
+        <v>0</v>
+      </c>
       <c r="N9" s="16">
-        <f>SUM(N6:N8)</f>
-        <v>0</v>
-      </c>
-      <c r="O9" s="16">
-        <f t="shared" ref="O9" si="3">SUM(O6:O8)</f>
-        <v>0</v>
+        <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="P9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="Q9" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -3359,14 +2934,13 @@
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
+      <c r="H10" s="16">
+        <f>SUM(C10:G10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -3385,13 +2959,10 @@
       <c r="G11" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I11" s="16"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -3410,13 +2981,10 @@
       <c r="G12" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="16"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -3427,14 +2995,13 @@
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="H13" s="16">
+        <f>SUM(C13:G13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -3443,14 +3010,13 @@
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
+      <c r="H14" s="16">
+        <f>SUM(C14:G14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -3469,13 +3035,10 @@
       <c r="G15" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" s="16"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -3494,19 +3057,16 @@
       <c r="G16" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I16" s="16"/>
+      <c r="H16" s="16"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="D25" sqref="D25"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F28" sqref="F28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="D25" sqref="D25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -3520,4 +3080,1198 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10" customWidth="1"/>
+    <col min="15" max="16" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="20">
+        <v>43027</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="9">
+        <f>B1</f>
+        <v>43027</v>
+      </c>
+      <c r="D3" s="9">
+        <f>C3+1</f>
+        <v>43028</v>
+      </c>
+      <c r="E3" s="9">
+        <f>D3+3</f>
+        <v>43031</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:G3" si="0">E3+1</f>
+        <v>43032</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="0"/>
+        <v>43033</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="10" t="str">
+        <f>TEXT(C3,"DDDD")</f>
+        <v>Thursday</v>
+      </c>
+      <c r="D4" s="10" t="str">
+        <f t="shared" ref="D4:G4" si="1">TEXT(D3,"DDDD")</f>
+        <v>Friday</v>
+      </c>
+      <c r="E4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Monday</v>
+      </c>
+      <c r="F4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="G4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
+        <f>SUM(C5:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16">
+        <f>SUM(C6:G6)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16">
+        <f>H5</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="16">
+        <f>H6</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="29"/>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="L7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="16">
+        <f>H9</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="16">
+        <f>H10</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="L8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="16">
+        <f>H13</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="16">
+        <f>H14</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16">
+        <f>SUM(C9:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="16">
+        <f>SUM(M6:M8)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="16">
+        <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16">
+        <f>SUM(C10:G10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16">
+        <f>SUM(C13:G13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16">
+        <f>SUM(C14:G14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10" customWidth="1"/>
+    <col min="15" max="16" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="20">
+        <v>43034</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="9">
+        <f>B1</f>
+        <v>43034</v>
+      </c>
+      <c r="D3" s="9">
+        <f>C3+1</f>
+        <v>43035</v>
+      </c>
+      <c r="E3" s="9">
+        <f>D3+3</f>
+        <v>43038</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:G3" si="0">E3+1</f>
+        <v>43039</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="0"/>
+        <v>43040</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="10" t="str">
+        <f>TEXT(C3,"DDDD")</f>
+        <v>Thursday</v>
+      </c>
+      <c r="D4" s="10" t="str">
+        <f t="shared" ref="D4:G4" si="1">TEXT(D3,"DDDD")</f>
+        <v>Friday</v>
+      </c>
+      <c r="E4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Monday</v>
+      </c>
+      <c r="F4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="G4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
+        <f>SUM(C5:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16">
+        <f>SUM(C6:G6)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16">
+        <f>H5</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="16">
+        <f>H6</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="29"/>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="L7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="16">
+        <f>H9</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="16">
+        <f>H10</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="L8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="16">
+        <f>H13</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="16">
+        <f>H14</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16">
+        <f>SUM(C9:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="16">
+        <f>SUM(M6:M8)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="16">
+        <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16">
+        <f>SUM(C10:G10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16">
+        <f>SUM(C13:G13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16">
+        <f>SUM(C14:G14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10" customWidth="1"/>
+    <col min="15" max="16" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="20">
+        <v>43041</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="9">
+        <f>B1</f>
+        <v>43041</v>
+      </c>
+      <c r="D3" s="9">
+        <f>C3+1</f>
+        <v>43042</v>
+      </c>
+      <c r="E3" s="9">
+        <f>D3+3</f>
+        <v>43045</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:G3" si="0">E3+1</f>
+        <v>43046</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="0"/>
+        <v>43047</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="10" t="str">
+        <f>TEXT(C3,"DDDD")</f>
+        <v>Thursday</v>
+      </c>
+      <c r="D4" s="10" t="str">
+        <f t="shared" ref="D4:G4" si="1">TEXT(D3,"DDDD")</f>
+        <v>Friday</v>
+      </c>
+      <c r="E4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Monday</v>
+      </c>
+      <c r="F4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="G4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
+        <f>SUM(C5:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16">
+        <f>SUM(C6:G6)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16">
+        <f>H5</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="16">
+        <f>H6</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="29"/>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="L7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="16">
+        <f>H9</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="16">
+        <f>H10</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="L8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="16">
+        <f>H13</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="16">
+        <f>H14</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16">
+        <f>SUM(C9:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="16">
+        <f>SUM(M6:M8)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="16">
+        <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16">
+        <f>SUM(C10:G10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16">
+        <f>SUM(C13:G13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16">
+        <f>SUM(C14:G14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated added wed ticket
</commit_message>
<xml_diff>
--- a/Ticket_Tally_Sheet.xlsx
+++ b/Ticket_Tally_Sheet.xlsx
@@ -23,9 +23,9 @@
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
+    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
     <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="4"/>
-    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
-    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1222,7 +1222,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1232,7 +1232,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1732,7 +1732,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1742,7 +1742,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2207,13 +2207,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -2232,8 +2232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="M8" s="16">
         <f>H13</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N8" s="16">
         <f>H14</f>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="M9" s="16">
         <f>SUM(M6:M8)</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N9" s="16">
         <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
@@ -2592,10 +2592,12 @@
       <c r="F13" s="16">
         <v>3</v>
       </c>
-      <c r="G13" s="16"/>
+      <c r="G13" s="16">
+        <v>2</v>
+      </c>
       <c r="H13" s="16">
         <f>SUM(C13:G13)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -2615,7 +2617,9 @@
       <c r="F14" s="16">
         <v>0</v>
       </c>
-      <c r="G14" s="16"/>
+      <c r="G14" s="16">
+        <v>0</v>
+      </c>
       <c r="H14" s="16">
         <f>SUM(C14:G14)</f>
         <v>2</v>
@@ -2667,13 +2671,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="I31" sqref="I31"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="E24" sqref="E24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="I31" sqref="I31"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -3077,13 +3081,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="D25" sqref="D25"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F28" sqref="F28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F28" sqref="F28"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="D25" sqref="D25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>

</xml_diff>

<commit_message>
Added values for 10/12 week.
</commit_message>
<xml_diff>
--- a/Ticket_Tally_Sheet.xlsx
+++ b/Ticket_Tally_Sheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SSIS-Shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SSIS\SSIS-Shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Tally_20170914" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,9 @@
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="4"/>
+    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
     <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
-    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
-    <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1222,7 +1222,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1232,7 +1232,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1732,7 +1732,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1742,7 +1742,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2207,13 +2207,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -2232,8 +2232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2675,13 +2675,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="E24" sqref="E24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="I31" sqref="I31"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="I31" sqref="I31"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -2700,8 +2700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E24:E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2862,11 +2862,11 @@
       </c>
       <c r="M7" s="16">
         <f>H9</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N7" s="16">
         <f>H10</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O7" s="16" t="s">
         <v>6</v>
@@ -2921,25 +2921,35 @@
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="C9" s="16">
+        <v>3</v>
+      </c>
+      <c r="D9" s="16">
+        <v>4</v>
+      </c>
+      <c r="E9" s="16">
+        <v>2</v>
+      </c>
+      <c r="F9" s="16">
+        <v>3</v>
+      </c>
+      <c r="G9" s="16">
+        <v>4</v>
+      </c>
       <c r="H9" s="16">
         <f>SUM(C9:G9)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L9" s="23" t="s">
         <v>8</v>
       </c>
       <c r="M9" s="16">
         <f>SUM(M6:M8)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N9" s="16">
         <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O9" s="16" t="s">
         <v>6</v>
@@ -2953,14 +2963,24 @@
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+      <c r="C10" s="16">
+        <v>2</v>
+      </c>
+      <c r="D10" s="16">
+        <v>4</v>
+      </c>
+      <c r="E10" s="16">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16">
+        <v>1</v>
+      </c>
+      <c r="G10" s="16">
+        <v>4</v>
+      </c>
       <c r="H10" s="16">
         <f>SUM(C10:G10)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -3085,13 +3105,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F28" sqref="F28"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="D25" sqref="D25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="D25" sqref="D25"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F28" sqref="F28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>

</xml_diff>

<commit_message>
Added values to 10/26 period
</commit_message>
<xml_diff>
--- a/Ticket_Tally_Sheet.xlsx
+++ b/Ticket_Tally_Sheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSIS-Shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SSIS\SSIS-Shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Tally_20170914" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,9 @@
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
+    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
     <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="4"/>
-    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
-    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1226,7 +1226,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1236,7 +1236,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1736,7 +1736,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1746,7 +1746,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2211,13 +2211,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -2679,13 +2679,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="I31" sqref="I31"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="E24" sqref="E24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="I31" sqref="I31"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -3149,13 +3149,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="D25" sqref="D25"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F28" sqref="F28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F28" sqref="F28"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="D25" sqref="D25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -3174,7 +3174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -3624,8 +3624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3786,11 +3786,11 @@
       </c>
       <c r="M7" s="16">
         <f>H9</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="N7" s="16">
         <f>H10</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="O7" s="16" t="s">
         <v>6</v>
@@ -3846,32 +3846,34 @@
         <v>2</v>
       </c>
       <c r="C9" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9" s="16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E9" s="16">
         <v>0</v>
       </c>
       <c r="F9" s="16">
-        <v>3</v>
-      </c>
-      <c r="G9" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="16">
+        <v>0</v>
+      </c>
       <c r="H9" s="16">
         <f>SUM(C9:G9)</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="L9" s="23" t="s">
         <v>8</v>
       </c>
       <c r="M9" s="16">
         <f>SUM(M6:M8)</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="N9" s="16">
         <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="O9" s="16" t="s">
         <v>6</v>
@@ -3886,21 +3888,23 @@
         <v>3</v>
       </c>
       <c r="C10" s="16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E10" s="16">
         <v>0</v>
       </c>
       <c r="F10" s="16">
-        <v>2</v>
-      </c>
-      <c r="G10" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="16">
+        <v>0</v>
+      </c>
       <c r="H10" s="16">
         <f>SUM(C10:G10)</f>
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added values to 11/2 week
</commit_message>
<xml_diff>
--- a/Ticket_Tally_Sheet.xlsx
+++ b/Ticket_Tally_Sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Tally_20170914" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,9 @@
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="4"/>
+    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
     <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
-    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
-    <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1226,7 +1226,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1236,7 +1236,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1736,7 +1736,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1746,7 +1746,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2211,13 +2211,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -2679,13 +2679,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="E24" sqref="E24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="I31" sqref="I31"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="I31" sqref="I31"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -3149,13 +3149,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F28" sqref="F28"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="D25" sqref="D25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="D25" sqref="D25"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F28" sqref="F28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -3624,7 +3624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -4042,8 +4042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4204,11 +4204,11 @@
       </c>
       <c r="M7" s="16">
         <f>H9</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="N7" s="16">
         <f>H10</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O7" s="16" t="s">
         <v>6</v>
@@ -4263,25 +4263,35 @@
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="C9" s="16">
+        <v>7</v>
+      </c>
+      <c r="D9" s="16">
+        <v>3</v>
+      </c>
+      <c r="E9" s="16">
+        <v>5</v>
+      </c>
+      <c r="F9" s="16">
+        <v>4</v>
+      </c>
+      <c r="G9" s="16">
+        <v>3</v>
+      </c>
       <c r="H9" s="16">
         <f>SUM(C9:G9)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="L9" s="23" t="s">
         <v>8</v>
       </c>
       <c r="M9" s="16">
         <f>SUM(M6:M8)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="N9" s="16">
         <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O9" s="16" t="s">
         <v>6</v>
@@ -4295,14 +4305,24 @@
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+      <c r="C10" s="16">
+        <v>5</v>
+      </c>
+      <c r="D10" s="16">
+        <v>3</v>
+      </c>
+      <c r="E10" s="16">
+        <v>4</v>
+      </c>
+      <c r="F10" s="16">
+        <v>1</v>
+      </c>
+      <c r="G10" s="16">
+        <v>1</v>
+      </c>
       <c r="H10" s="16">
         <f>SUM(C10:G10)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added values for 11/9 week.
</commit_message>
<xml_diff>
--- a/Ticket_Tally_Sheet.xlsx
+++ b/Ticket_Tally_Sheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSIS-Shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SSIS\SSIS-Shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Tally_20170914" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,13 @@
     <sheet name="Tally_20171019" sheetId="6" r:id="rId6"/>
     <sheet name="Tally_20171026" sheetId="7" r:id="rId7"/>
     <sheet name="Tally_20171102" sheetId="8" r:id="rId8"/>
-    <sheet name="Tally_20171019 (2)" sheetId="9" r:id="rId9"/>
+    <sheet name="Tally_20171109" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="4"/>
+    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
     <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
-    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
-    <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1226,7 +1226,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1236,7 +1236,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1736,7 +1736,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1746,7 +1746,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2211,13 +2211,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -2679,13 +2679,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="E24" sqref="E24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="I31" sqref="I31"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="I31" sqref="I31"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -3149,13 +3149,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F28" sqref="F28"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="D25" sqref="D25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="D25" sqref="D25"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F28" sqref="F28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -3175,7 +3175,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C5" sqref="C5:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3624,7 +3624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -4520,8 +4520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4540,7 +4540,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="20">
-        <v>43034</v>
+        <v>43048</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -4550,23 +4550,23 @@
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C3" s="9">
         <f>B1</f>
-        <v>43034</v>
+        <v>43048</v>
       </c>
       <c r="D3" s="9">
         <f>C3+1</f>
-        <v>43035</v>
+        <v>43049</v>
       </c>
       <c r="E3" s="9">
         <f>D3+3</f>
-        <v>43038</v>
+        <v>43052</v>
       </c>
       <c r="F3" s="9">
         <f t="shared" ref="F3:G3" si="0">E3+1</f>
-        <v>43039</v>
+        <v>43053</v>
       </c>
       <c r="G3" s="9">
         <f t="shared" si="0"/>
-        <v>43040</v>
+        <v>43054</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -4601,14 +4601,24 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="C5" s="16">
+        <v>2</v>
+      </c>
+      <c r="D5" s="16">
+        <v>2</v>
+      </c>
+      <c r="E5" s="16">
+        <v>1</v>
+      </c>
+      <c r="F5" s="16">
+        <v>1</v>
+      </c>
+      <c r="G5" s="16">
+        <v>0</v>
+      </c>
       <c r="H5" s="16">
         <f>SUM(C5:G5)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="26" t="s">
@@ -4629,11 +4639,21 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
+      <c r="C6" s="16">
+        <v>0</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0</v>
+      </c>
       <c r="H6" s="16">
         <f>SUM(C6:G6)</f>
         <v>0</v>
@@ -4643,7 +4663,7 @@
       </c>
       <c r="M6" s="16">
         <f>H5</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N6" s="16">
         <f>H6</f>
@@ -4682,11 +4702,11 @@
       </c>
       <c r="M7" s="16">
         <f>H9</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N7" s="16">
         <f>H10</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O7" s="16" t="s">
         <v>6</v>
@@ -4721,7 +4741,7 @@
       </c>
       <c r="M8" s="16">
         <f>H13</f>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="N8" s="16">
         <f>H14</f>
@@ -4742,32 +4762,34 @@
         <v>2</v>
       </c>
       <c r="C9" s="16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" s="16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="16">
         <v>3</v>
       </c>
-      <c r="G9" s="16"/>
+      <c r="G9" s="16">
+        <v>4</v>
+      </c>
       <c r="H9" s="16">
         <f>SUM(C9:G9)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L9" s="23" t="s">
         <v>8</v>
       </c>
       <c r="M9" s="16">
         <f>SUM(M6:M8)</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="N9" s="16">
         <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="O9" s="16" t="s">
         <v>6</v>
@@ -4782,21 +4804,23 @@
         <v>3</v>
       </c>
       <c r="C10" s="16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D10" s="16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E10" s="16">
         <v>0</v>
       </c>
       <c r="F10" s="16">
-        <v>2</v>
-      </c>
-      <c r="G10" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="G10" s="16">
+        <v>3</v>
+      </c>
       <c r="H10" s="16">
         <f>SUM(C10:G10)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -4851,23 +4875,23 @@
         <v>2</v>
       </c>
       <c r="C13" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13" s="16">
         <v>3</v>
       </c>
       <c r="E13" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G13" s="16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H13" s="16">
         <f>SUM(C13:G13)</f>
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -4876,10 +4900,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="16">
         <v>0</v>
@@ -4888,7 +4912,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H14" s="16">
         <f>SUM(C14:G14)</f>

</xml_diff>

<commit_message>
Added values to 11/16 week.
</commit_message>
<xml_diff>
--- a/Ticket_Tally_Sheet.xlsx
+++ b/Ticket_Tally_Sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Tally_20170914" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,15 @@
     <sheet name="Tally_20171026" sheetId="7" r:id="rId7"/>
     <sheet name="Tally_20171102" sheetId="8" r:id="rId8"/>
     <sheet name="Tally_20171109" sheetId="9" r:id="rId9"/>
+    <sheet name="Tally_20171116" sheetId="10" r:id="rId10"/>
+    <sheet name="Tally_20171123" sheetId="11" r:id="rId11"/>
+    <sheet name="Tally_20171130" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
+    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
     <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="4"/>
-    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
-    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="10">
   <si>
     <t>Benson Fabonan</t>
   </si>
@@ -342,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -398,6 +401,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -824,7 +830,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -865,7 +871,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="7" t="s">
         <v>3</v>
       </c>
@@ -908,7 +914,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -950,7 +956,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
@@ -992,7 +998,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -1039,7 +1045,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="7" t="s">
         <v>3</v>
       </c>
@@ -1067,7 +1073,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="7" t="s">
         <v>4</v>
       </c>
@@ -1092,7 +1098,7 @@
       <c r="I11" s="12"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="29"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="8" t="s">
         <v>5</v>
       </c>
@@ -1117,7 +1123,7 @@
       <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="28" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -1147,7 +1153,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="7" t="s">
         <v>3</v>
       </c>
@@ -1175,7 +1181,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="7" t="s">
         <v>4</v>
       </c>
@@ -1200,7 +1206,7 @@
       <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="29"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="8" t="s">
         <v>5</v>
       </c>
@@ -1226,7 +1232,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1236,7 +1242,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1252,6 +1258,1220 @@
   <ignoredErrors>
     <ignoredError sqref="E3" formula="1"/>
   </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10" customWidth="1"/>
+    <col min="15" max="16" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="20">
+        <v>43055</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="9">
+        <f>B1</f>
+        <v>43055</v>
+      </c>
+      <c r="D3" s="9">
+        <f>C3+1</f>
+        <v>43056</v>
+      </c>
+      <c r="E3" s="9">
+        <f>D3+3</f>
+        <v>43059</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:G3" si="0">E3+1</f>
+        <v>43060</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="0"/>
+        <v>43061</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="10" t="str">
+        <f>TEXT(C3,"DDDD")</f>
+        <v>Thursday</v>
+      </c>
+      <c r="D4" s="10" t="str">
+        <f t="shared" ref="D4:G4" si="1">TEXT(D3,"DDDD")</f>
+        <v>Friday</v>
+      </c>
+      <c r="E4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Monday</v>
+      </c>
+      <c r="F4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="G4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
+        <f>SUM(C5:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16">
+        <f>SUM(C6:G6)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16">
+        <f>H5</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="16">
+        <f>H6</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="L7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="16">
+        <f>H9</f>
+        <v>14</v>
+      </c>
+      <c r="N7" s="16">
+        <f>H10</f>
+        <v>10</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="L8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="16">
+        <f>H13</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="16">
+        <f>H14</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="16">
+        <v>4</v>
+      </c>
+      <c r="D9" s="16">
+        <v>5</v>
+      </c>
+      <c r="E9" s="16">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16">
+        <v>0</v>
+      </c>
+      <c r="G9" s="16">
+        <v>4</v>
+      </c>
+      <c r="H9" s="16">
+        <f>SUM(C9:G9)</f>
+        <v>14</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="16">
+        <f>SUM(M6:M8)</f>
+        <v>14</v>
+      </c>
+      <c r="N9" s="16">
+        <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
+        <v>10</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="16">
+        <v>2</v>
+      </c>
+      <c r="D10" s="16">
+        <v>3</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0</v>
+      </c>
+      <c r="F10" s="16">
+        <v>1</v>
+      </c>
+      <c r="G10" s="16">
+        <v>4</v>
+      </c>
+      <c r="H10" s="16">
+        <f>SUM(C10:G10)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16">
+        <f>SUM(C13:G13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16">
+        <f>SUM(C14:G14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="31"/>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10" customWidth="1"/>
+    <col min="15" max="16" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="20">
+        <v>43062</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="9">
+        <f>B1</f>
+        <v>43062</v>
+      </c>
+      <c r="D3" s="9">
+        <f>C3+1</f>
+        <v>43063</v>
+      </c>
+      <c r="E3" s="9">
+        <f>D3+3</f>
+        <v>43066</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:G3" si="0">E3+1</f>
+        <v>43067</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="0"/>
+        <v>43068</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="10" t="str">
+        <f>TEXT(C3,"DDDD")</f>
+        <v>Thursday</v>
+      </c>
+      <c r="D4" s="10" t="str">
+        <f t="shared" ref="D4:G4" si="1">TEXT(D3,"DDDD")</f>
+        <v>Friday</v>
+      </c>
+      <c r="E4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Monday</v>
+      </c>
+      <c r="F4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="G4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
+        <f>SUM(C5:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16">
+        <f>SUM(C6:G6)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16">
+        <f>H5</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="16">
+        <f>H6</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="L7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="16">
+        <f>H9</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="16">
+        <f>H10</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="L8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="16">
+        <f>H13</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="16">
+        <f>H14</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16">
+        <f>SUM(C9:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="16">
+        <f>SUM(M6:M8)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="16">
+        <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16">
+        <f>SUM(C10:G10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16">
+        <f>SUM(C13:G13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16">
+        <f>SUM(C14:G14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="31"/>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10" customWidth="1"/>
+    <col min="15" max="16" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="20">
+        <v>43069</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="9">
+        <f>B1</f>
+        <v>43069</v>
+      </c>
+      <c r="D3" s="9">
+        <f>C3+1</f>
+        <v>43070</v>
+      </c>
+      <c r="E3" s="9">
+        <f>D3+3</f>
+        <v>43073</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:G3" si="0">E3+1</f>
+        <v>43074</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="0"/>
+        <v>43075</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="10" t="str">
+        <f>TEXT(C3,"DDDD")</f>
+        <v>Thursday</v>
+      </c>
+      <c r="D4" s="10" t="str">
+        <f t="shared" ref="D4:G4" si="1">TEXT(D3,"DDDD")</f>
+        <v>Friday</v>
+      </c>
+      <c r="E4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Monday</v>
+      </c>
+      <c r="F4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="G4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
+        <f>SUM(C5:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16">
+        <f>SUM(C6:G6)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16">
+        <f>H5</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="16">
+        <f>H6</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="L7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="16">
+        <f>H9</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="16">
+        <f>H10</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="L8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="16">
+        <f>H13</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="16">
+        <f>H14</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16">
+        <f>SUM(C9:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="16">
+        <f>SUM(M6:M8)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="16">
+        <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16">
+        <f>SUM(C10:G10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16">
+        <f>SUM(C13:G13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16">
+        <f>SUM(C14:G14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="31"/>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1342,7 +2562,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1381,7 +2601,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1422,7 +2642,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1464,7 +2684,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1506,7 +2726,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1553,7 +2773,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1581,7 +2801,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1606,7 +2826,7 @@
       <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1631,7 +2851,7 @@
       <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="31" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1659,7 +2879,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1685,7 +2905,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1710,7 +2930,7 @@
       <c r="I15" s="16"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1736,7 +2956,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1746,7 +2966,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1841,7 +3061,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1881,7 +3101,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1923,7 +3143,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1962,7 +3182,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2001,7 +3221,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2045,7 +3265,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -2070,7 +3290,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -2092,7 +3312,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -2114,7 +3334,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="31" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2141,7 +3361,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -2166,7 +3386,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2188,7 +3408,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -2211,13 +3431,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -2311,7 +3531,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2351,7 +3571,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2393,7 +3613,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2432,7 +3652,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2471,7 +3691,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2515,7 +3735,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -2538,7 +3758,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -2560,7 +3780,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -2582,7 +3802,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="31" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2609,7 +3829,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -2634,7 +3854,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2656,7 +3876,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -2679,13 +3899,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="I31" sqref="I31"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="E24" sqref="E24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="I31" sqref="I31"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -2779,7 +3999,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2819,7 +4039,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2861,7 +4081,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2900,7 +4120,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2939,7 +4159,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2983,7 +4203,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -3008,7 +4228,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -3030,7 +4250,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -3052,7 +4272,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="31" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -3079,7 +4299,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -3104,7 +4324,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -3126,7 +4346,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -3149,13 +4369,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="D25" sqref="D25"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F28" sqref="F28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F28" sqref="F28"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="D25" sqref="D25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -3249,7 +4469,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3287,7 +4507,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3327,7 +4547,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3366,7 +4586,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3405,7 +4625,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -3447,7 +4667,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -3470,7 +4690,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -3492,7 +4712,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -3514,7 +4734,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="31" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -3541,7 +4761,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -3566,7 +4786,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -3588,7 +4808,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -3699,7 +4919,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3729,7 +4949,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3761,7 +4981,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3800,7 +5020,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3839,7 +5059,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -3883,7 +5103,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -3908,7 +5128,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -3930,7 +5150,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -3952,7 +5172,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="31" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -3979,7 +5199,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -4004,7 +5224,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -4026,7 +5246,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -4137,7 +5357,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -4177,7 +5397,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4219,7 +5439,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4258,7 +5478,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4297,7 +5517,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -4341,7 +5561,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -4366,7 +5586,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -4388,7 +5608,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -4410,7 +5630,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="31" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -4437,7 +5657,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -4462,7 +5682,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -4484,7 +5704,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -4520,7 +5740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -4595,7 +5815,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -4635,7 +5855,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4677,7 +5897,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4716,7 +5936,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4755,7 +5975,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -4799,7 +6019,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -4824,7 +6044,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -4846,7 +6066,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -4868,7 +6088,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="31" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -4895,7 +6115,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -4920,7 +6140,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -4942,7 +6162,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Added entry for 11/22
</commit_message>
<xml_diff>
--- a/Ticket_Tally_Sheet.xlsx
+++ b/Ticket_Tally_Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSIS-Shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SSIS-Shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,9 +27,9 @@
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="4"/>
+    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
     <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
-    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
-    <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1232,7 +1232,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1242,7 +1242,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1266,7 +1266,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,14 +1346,24 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="C5" s="16">
+        <v>5</v>
+      </c>
+      <c r="D5" s="16">
+        <v>1</v>
+      </c>
+      <c r="E5" s="16">
+        <v>2</v>
+      </c>
+      <c r="F5" s="16">
+        <v>0</v>
+      </c>
+      <c r="G5" s="16">
+        <v>1</v>
+      </c>
       <c r="H5" s="16">
         <f>SUM(C5:G5)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="27" t="s">
@@ -1374,25 +1384,35 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
+      <c r="C6" s="16">
+        <v>2</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16">
+        <v>2</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0</v>
+      </c>
       <c r="H6" s="16">
         <f>SUM(C6:G6)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="M6" s="16">
         <f>H5</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="N6" s="16">
         <f>H6</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O6" s="16" t="s">
         <v>6</v>
@@ -1510,11 +1530,11 @@
       </c>
       <c r="M9" s="16">
         <f>SUM(M6:M8)</f>
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="N9" s="16">
         <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="O9" s="16" t="s">
         <v>6</v>
@@ -2976,7 +2996,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2986,7 +3006,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -3451,13 +3471,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -3919,13 +3939,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="E24" sqref="E24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="I31" sqref="I31"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="I31" sqref="I31"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -4389,13 +4409,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F28" sqref="F28"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="D25" sqref="D25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="D25" sqref="D25"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F28" sqref="F28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>

</xml_diff>

<commit_message>
Added values to 11/23 week.
</commit_message>
<xml_diff>
--- a/Ticket_Tally_Sheet.xlsx
+++ b/Ticket_Tally_Sheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SSIS-Shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SSIS\SSIS-Shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Tally_20170914" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,9 @@
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
+    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
     <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="4"/>
-    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
-    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1232,7 +1232,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1242,7 +1242,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1265,7 +1265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1723,8 +1723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1885,11 +1885,11 @@
       </c>
       <c r="M7" s="16">
         <f>H9</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N7" s="16">
         <f>H10</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O7" s="16" t="s">
         <v>6</v>
@@ -1944,25 +1944,35 @@
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="C9" s="16">
+        <v>4</v>
+      </c>
+      <c r="D9" s="16">
+        <v>2</v>
+      </c>
+      <c r="E9" s="16">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16">
+        <v>2</v>
+      </c>
+      <c r="G9" s="16">
+        <v>5</v>
+      </c>
       <c r="H9" s="16">
         <f>SUM(C9:G9)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L9" s="23" t="s">
         <v>8</v>
       </c>
       <c r="M9" s="16">
         <f>SUM(M6:M8)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N9" s="16">
         <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O9" s="16" t="s">
         <v>6</v>
@@ -1976,14 +1986,24 @@
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+      <c r="C10" s="16">
+        <v>3</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0</v>
+      </c>
+      <c r="F10" s="16">
+        <v>0</v>
+      </c>
+      <c r="G10" s="16">
+        <v>0</v>
+      </c>
       <c r="H10" s="16">
         <f>SUM(C10:G10)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2996,7 +3016,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3006,7 +3026,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -3471,13 +3491,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -3939,13 +3959,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="I31" sqref="I31"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="E24" sqref="E24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="I31" sqref="I31"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -4409,13 +4429,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="D25" sqref="D25"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F28" sqref="F28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F28" sqref="F28"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="D25" sqref="D25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>

</xml_diff>

<commit_message>
Added values to 11/30 week.
</commit_message>
<xml_diff>
--- a/Ticket_Tally_Sheet.xlsx
+++ b/Ticket_Tally_Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSIS-Shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SSIS\SSIS-Shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,12 +24,16 @@
     <sheet name="Tally_20171116" sheetId="10" r:id="rId10"/>
     <sheet name="Tally_20171123" sheetId="11" r:id="rId11"/>
     <sheet name="Tally_20171130" sheetId="12" r:id="rId12"/>
+    <sheet name="Tally_20171207" sheetId="13" r:id="rId13"/>
+    <sheet name="Tally_20171214" sheetId="14" r:id="rId14"/>
+    <sheet name="Tally_20171221" sheetId="15" r:id="rId15"/>
+    <sheet name="Tally_20171228" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
+    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
     <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="4"/>
-    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
-    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="10">
   <si>
     <t>Benson Fabonan</t>
   </si>
@@ -345,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -401,6 +405,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -830,7 +837,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -871,7 +878,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="7" t="s">
         <v>3</v>
       </c>
@@ -914,7 +921,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -956,7 +963,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
@@ -998,7 +1005,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -1045,7 +1052,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="7" t="s">
         <v>3</v>
       </c>
@@ -1073,7 +1080,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="7" t="s">
         <v>4</v>
       </c>
@@ -1098,7 +1105,7 @@
       <c r="I11" s="12"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="8" t="s">
         <v>5</v>
       </c>
@@ -1123,7 +1130,7 @@
       <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -1153,7 +1160,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="7" t="s">
         <v>3</v>
       </c>
@@ -1181,7 +1188,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="7" t="s">
         <v>4</v>
       </c>
@@ -1206,7 +1213,7 @@
       <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="30"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="8" t="s">
         <v>5</v>
       </c>
@@ -1232,7 +1239,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1242,7 +1249,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1340,7 +1347,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1380,7 +1387,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1422,7 +1429,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1461,7 +1468,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1500,7 +1507,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1544,7 +1551,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1569,7 +1576,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1591,7 +1598,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1613,7 +1620,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1640,7 +1647,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1665,7 +1672,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1687,7 +1694,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1798,7 +1805,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1838,7 +1845,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1880,7 +1887,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1919,7 +1926,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1958,7 +1965,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2002,7 +2009,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -2027,7 +2034,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -2049,7 +2056,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -2071,7 +2078,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2098,7 +2105,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -2123,7 +2130,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2145,7 +2152,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -2182,7 +2189,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,7 +2263,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2286,7 +2293,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2318,7 +2325,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2343,11 +2350,11 @@
       </c>
       <c r="M7" s="16">
         <f>H9</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="N7" s="16">
         <f>H10</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O7" s="16" t="s">
         <v>6</v>
@@ -2357,7 +2364,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2396,7 +2403,445 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="16">
+        <v>2</v>
+      </c>
+      <c r="D9" s="16">
+        <v>1</v>
+      </c>
+      <c r="E9" s="16">
+        <v>6</v>
+      </c>
+      <c r="F9" s="16">
+        <v>4</v>
+      </c>
+      <c r="G9" s="16">
+        <v>4</v>
+      </c>
+      <c r="H9" s="16">
+        <f>SUM(C9:G9)</f>
+        <v>17</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="16">
+        <f>SUM(M6:M8)</f>
+        <v>22</v>
+      </c>
+      <c r="N9" s="16">
+        <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
+        <v>17</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="16">
+        <v>0</v>
+      </c>
+      <c r="D10" s="16">
+        <v>2</v>
+      </c>
+      <c r="E10" s="16">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16">
+        <v>3</v>
+      </c>
+      <c r="G10" s="16">
+        <v>0</v>
+      </c>
+      <c r="H10" s="16">
+        <f>SUM(C10:G10)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="16">
+        <v>0</v>
+      </c>
+      <c r="D13" s="16">
+        <v>0</v>
+      </c>
+      <c r="E13" s="16">
+        <v>2</v>
+      </c>
+      <c r="F13" s="16">
+        <v>1</v>
+      </c>
+      <c r="G13" s="16">
+        <v>2</v>
+      </c>
+      <c r="H13" s="16">
+        <f>SUM(C13:G13)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="16">
+        <v>0</v>
+      </c>
+      <c r="D14" s="16">
+        <v>0</v>
+      </c>
+      <c r="E14" s="16">
+        <v>3</v>
+      </c>
+      <c r="F14" s="16">
+        <v>2</v>
+      </c>
+      <c r="G14" s="16">
+        <v>6</v>
+      </c>
+      <c r="H14" s="16">
+        <f>SUM(C14:G14)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10" customWidth="1"/>
+    <col min="15" max="16" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="20">
+        <v>43076</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="9">
+        <f>B1</f>
+        <v>43076</v>
+      </c>
+      <c r="D3" s="9">
+        <f>C3+1</f>
+        <v>43077</v>
+      </c>
+      <c r="E3" s="9">
+        <f>D3+3</f>
+        <v>43080</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:G3" si="0">E3+1</f>
+        <v>43081</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="0"/>
+        <v>43082</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="10" t="str">
+        <f>TEXT(C3,"DDDD")</f>
+        <v>Thursday</v>
+      </c>
+      <c r="D4" s="10" t="str">
+        <f t="shared" ref="D4:G4" si="1">TEXT(D3,"DDDD")</f>
+        <v>Friday</v>
+      </c>
+      <c r="E4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Monday</v>
+      </c>
+      <c r="F4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="G4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
+        <f>SUM(C5:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16">
+        <f>SUM(C6:G6)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16">
+        <f>H5</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="16">
+        <f>H6</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="L7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="16">
+        <f>H9</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="16">
+        <f>H10</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="L8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="16">
+        <f>H13</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="16">
+        <f>H14</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2416,11 +2861,11 @@
       </c>
       <c r="M9" s="16">
         <f>SUM(M6:M8)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N9" s="16">
         <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="O9" s="16" t="s">
         <v>6</v>
@@ -2430,7 +2875,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -2445,7 +2890,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -2467,7 +2912,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -2489,59 +2934,39 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="16">
-        <v>0</v>
-      </c>
-      <c r="D13" s="16">
-        <v>0</v>
-      </c>
-      <c r="E13" s="16">
-        <v>2</v>
-      </c>
-      <c r="F13" s="16">
-        <v>1</v>
-      </c>
-      <c r="G13" s="16">
-        <v>2</v>
-      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="16">
         <f>SUM(C13:G13)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="16">
-        <v>0</v>
-      </c>
-      <c r="D14" s="16">
-        <v>0</v>
-      </c>
-      <c r="E14" s="16">
-        <v>3</v>
-      </c>
-      <c r="F14" s="16">
-        <v>2</v>
-      </c>
-      <c r="G14" s="16">
-        <v>6</v>
-      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="16">
         <f>SUM(C14:G14)</f>
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2563,7 +2988,1201 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10" customWidth="1"/>
+    <col min="15" max="16" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="20">
+        <v>43083</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="9">
+        <f>B1</f>
+        <v>43083</v>
+      </c>
+      <c r="D3" s="9">
+        <f>C3+1</f>
+        <v>43084</v>
+      </c>
+      <c r="E3" s="9">
+        <f>D3+3</f>
+        <v>43087</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:G3" si="0">E3+1</f>
+        <v>43088</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="0"/>
+        <v>43089</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="10" t="str">
+        <f>TEXT(C3,"DDDD")</f>
+        <v>Thursday</v>
+      </c>
+      <c r="D4" s="10" t="str">
+        <f t="shared" ref="D4:G4" si="1">TEXT(D3,"DDDD")</f>
+        <v>Friday</v>
+      </c>
+      <c r="E4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Monday</v>
+      </c>
+      <c r="F4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="G4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
+        <f>SUM(C5:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16">
+        <f>SUM(C6:G6)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16">
+        <f>H5</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="16">
+        <f>H6</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="L7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="16">
+        <f>H9</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="16">
+        <f>H10</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="L8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="16">
+        <f>H13</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="16">
+        <f>H14</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16">
+        <f>SUM(C9:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="16">
+        <f>SUM(M6:M8)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="16">
+        <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16">
+        <f>SUM(C10:G10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16">
+        <f>SUM(C13:G13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16">
+        <f>SUM(C14:G14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10" customWidth="1"/>
+    <col min="15" max="16" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="20">
+        <v>43090</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="9">
+        <f>B1</f>
+        <v>43090</v>
+      </c>
+      <c r="D3" s="9">
+        <f>C3+1</f>
+        <v>43091</v>
+      </c>
+      <c r="E3" s="9">
+        <f>D3+3</f>
+        <v>43094</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:G3" si="0">E3+1</f>
+        <v>43095</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="0"/>
+        <v>43096</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="10" t="str">
+        <f>TEXT(C3,"DDDD")</f>
+        <v>Thursday</v>
+      </c>
+      <c r="D4" s="10" t="str">
+        <f t="shared" ref="D4:G4" si="1">TEXT(D3,"DDDD")</f>
+        <v>Friday</v>
+      </c>
+      <c r="E4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Monday</v>
+      </c>
+      <c r="F4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="G4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
+        <f>SUM(C5:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16">
+        <f>SUM(C6:G6)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16">
+        <f>H5</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="16">
+        <f>H6</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="L7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="16">
+        <f>H9</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="16">
+        <f>H10</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="L8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="16">
+        <f>H13</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="16">
+        <f>H14</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16">
+        <f>SUM(C9:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="16">
+        <f>SUM(M6:M8)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="16">
+        <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16">
+        <f>SUM(C10:G10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16">
+        <f>SUM(C13:G13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16">
+        <f>SUM(C14:G14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10" customWidth="1"/>
+    <col min="15" max="16" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="20">
+        <v>43097</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="9">
+        <f>B1</f>
+        <v>43097</v>
+      </c>
+      <c r="D3" s="9">
+        <f>C3+1</f>
+        <v>43098</v>
+      </c>
+      <c r="E3" s="9">
+        <f>D3+3</f>
+        <v>43101</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:G3" si="0">E3+1</f>
+        <v>43102</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="0"/>
+        <v>43103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="10" t="str">
+        <f>TEXT(C3,"DDDD")</f>
+        <v>Thursday</v>
+      </c>
+      <c r="D4" s="10" t="str">
+        <f t="shared" ref="D4:G4" si="1">TEXT(D3,"DDDD")</f>
+        <v>Friday</v>
+      </c>
+      <c r="E4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Monday</v>
+      </c>
+      <c r="F4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="G4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
+        <f>SUM(C5:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16">
+        <f>SUM(C6:G6)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16">
+        <f>H5</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="16">
+        <f>H6</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="L7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="16">
+        <f>H9</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="16">
+        <f>H10</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="L8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="16">
+        <f>H13</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="16">
+        <f>H14</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16">
+        <f>SUM(C9:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="16">
+        <f>SUM(M6:M8)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="16">
+        <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16">
+        <f>SUM(C10:G10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16">
+        <f>SUM(C13:G13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16">
+        <f>SUM(C14:G14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -2682,7 +4301,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2721,7 +4340,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2762,7 +4381,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2804,7 +4423,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2846,7 +4465,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2893,7 +4512,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -2921,7 +4540,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -2946,7 +4565,7 @@
       <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -2971,7 +4590,7 @@
       <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2999,7 +4618,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -3025,7 +4644,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -3050,7 +4669,7 @@
       <c r="I15" s="16"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -3076,7 +4695,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3086,7 +4705,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -3181,7 +4800,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3221,7 +4840,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3263,7 +4882,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3302,7 +4921,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3341,7 +4960,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -3385,7 +5004,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -3410,7 +5029,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -3432,7 +5051,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -3454,7 +5073,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -3481,7 +5100,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -3506,7 +5125,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -3528,7 +5147,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -3551,13 +5170,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -3651,7 +5270,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3691,7 +5310,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3733,7 +5352,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3772,7 +5391,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3811,7 +5430,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -3855,7 +5474,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -3878,7 +5497,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -3900,7 +5519,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -3922,7 +5541,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -3949,7 +5568,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -3974,7 +5593,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -3996,7 +5615,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -4019,13 +5638,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="I31" sqref="I31"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="E24" sqref="E24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="I31" sqref="I31"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -4119,7 +5738,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -4159,7 +5778,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4201,7 +5820,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4240,7 +5859,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4279,7 +5898,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -4323,7 +5942,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -4348,7 +5967,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -4370,7 +5989,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -4392,7 +6011,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -4419,7 +6038,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -4444,7 +6063,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -4466,7 +6085,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -4489,13 +6108,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="D25" sqref="D25"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F28" sqref="F28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F28" sqref="F28"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="D25" sqref="D25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -4589,7 +6208,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -4627,7 +6246,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4667,7 +6286,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4706,7 +6325,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4745,7 +6364,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -4787,7 +6406,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -4810,7 +6429,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -4832,7 +6451,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -4854,7 +6473,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -4881,7 +6500,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -4906,7 +6525,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -4928,7 +6547,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -5039,7 +6658,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -5069,7 +6688,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -5101,7 +6720,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5140,7 +6759,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -5179,7 +6798,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -5223,7 +6842,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -5248,7 +6867,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -5270,7 +6889,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -5292,7 +6911,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -5319,7 +6938,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -5344,7 +6963,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -5366,7 +6985,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -5477,7 +7096,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -5517,7 +7136,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -5559,7 +7178,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5598,7 +7217,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -5637,7 +7256,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -5681,7 +7300,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -5706,7 +7325,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -5728,7 +7347,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -5750,7 +7369,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -5777,7 +7396,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -5802,7 +7421,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -5824,7 +7443,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -5935,7 +7554,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -5975,7 +7594,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -6017,7 +7636,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -6056,7 +7675,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -6095,7 +7714,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -6139,7 +7758,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -6164,7 +7783,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -6186,7 +7805,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -6208,7 +7827,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -6235,7 +7854,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -6260,7 +7879,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -6282,7 +7901,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Added values for the week
</commit_message>
<xml_diff>
--- a/Ticket_Tally_Sheet.xlsx
+++ b/Ticket_Tally_Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSIS-Shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SSIS\SSIS-Shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,9 +31,9 @@
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
+    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
     <customWorkbookView name="Benson Fabonan - Personal View" guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="4"/>
-    <customWorkbookView name="Manuel Alberto Lomotan - Personal View" guid="{5DD559DC-FA50-4E4A-9646-8FEE718DD279}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" activeSheetId="2"/>
-    <customWorkbookView name="Jeric Ryan De Josef - Personal View" guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1019" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1239,7 +1239,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1249,7 +1249,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="L18" sqref="L18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2646,8 +2646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2808,11 +2808,11 @@
       </c>
       <c r="M7" s="16">
         <f>H9</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N7" s="16">
         <f>H10</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O7" s="16" t="s">
         <v>6</v>
@@ -2867,25 +2867,35 @@
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="C9" s="16">
+        <v>4</v>
+      </c>
+      <c r="D9" s="16">
+        <v>3</v>
+      </c>
+      <c r="E9" s="16">
+        <v>3</v>
+      </c>
+      <c r="F9" s="16">
+        <v>5</v>
+      </c>
+      <c r="G9" s="16">
+        <v>5</v>
+      </c>
       <c r="H9" s="16">
         <f>SUM(C9:G9)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L9" s="23" t="s">
         <v>8</v>
       </c>
       <c r="M9" s="16">
         <f>SUM(M6:M8)</f>
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="N9" s="16">
         <f t="shared" ref="N9" si="2">SUM(N6:N8)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="O9" s="16" t="s">
         <v>6</v>
@@ -2899,14 +2909,24 @@
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+      <c r="C10" s="16">
+        <v>2</v>
+      </c>
+      <c r="D10" s="16">
+        <v>1</v>
+      </c>
+      <c r="E10" s="16">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16">
+        <v>0</v>
+      </c>
+      <c r="G10" s="16">
+        <v>2</v>
+      </c>
       <c r="H10" s="16">
         <f>SUM(C10:G10)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -4735,7 +4755,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4745,7 +4765,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
       <selection activeCell="H11" sqref="H11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -5210,13 +5230,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -5678,13 +5698,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="I31" sqref="I31"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="E24" sqref="E24"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="I31" sqref="I31"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -6148,13 +6168,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
-      <selection activeCell="D25" sqref="D25"/>
+    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
+      <selection activeCell="F28" sqref="F28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{706D43D0-A44B-4E4B-BDBF-40C1EE9045CA}">
-      <selection activeCell="F28" sqref="F28"/>
+    <customSheetView guid="{6568F0E6-77C6-45C8-808D-B67B20EB14DF}">
+      <selection activeCell="D25" sqref="D25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>

</xml_diff>